<commit_message>
📊 Daily StockIQ Insights update (2026-01-08)
</commit_message>
<xml_diff>
--- a/Daily_StockIQ_Insights.xlsx
+++ b/Daily_StockIQ_Insights.xlsx
@@ -452,7 +452,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1692,683 +1692,1172 @@
         </is>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>RELIANCE.NS</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>1504.2</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1673.74</v>
+      </c>
+      <c r="F22" t="n">
+        <v>11.27</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1532.660034179688</v>
+      </c>
+      <c r="H22" t="n">
+        <v>1.889999985694885</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="J22" t="n">
+        <v>-0.784</v>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>⚠️ Cautious Buy</t>
+        </is>
+      </c>
+      <c r="M22" t="n">
+        <v>51.23</v>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>TCS.NS</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>3295.6</v>
+      </c>
+      <c r="E23" t="n">
+        <v>3263.94</v>
+      </c>
+      <c r="F23" t="n">
+        <v>-0.96</v>
+      </c>
+      <c r="G23" t="n">
+        <v>3285.1298828125</v>
+      </c>
+      <c r="H23" t="n">
+        <v>-0.3199999928474426</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J23" t="n">
+        <v>0.796</v>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="M23" t="n">
+        <v>64.48</v>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>INFY.NS</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>1639</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1637.55</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-0.09</v>
+      </c>
+      <c r="G24" t="n">
+        <v>1585.660034179688</v>
+      </c>
+      <c r="H24" t="n">
+        <v>-3.25</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J24" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="M24" t="n">
+        <v>62.87</v>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>HDFCBANK.NS</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>949.05</v>
+      </c>
+      <c r="E25" t="n">
+        <v>925.95</v>
+      </c>
+      <c r="F25" t="n">
+        <v>-2.43</v>
+      </c>
+      <c r="G25" t="n">
+        <v>907.719970703125</v>
+      </c>
+      <c r="H25" t="n">
+        <v>-4.349999904632568</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="J25" t="n">
+        <v>-0.65</v>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>❌ Strong Avoid</t>
+        </is>
+      </c>
+      <c r="M25" t="n">
+        <v>33.35</v>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>ICICIBANK.NS</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>1427.7</v>
+      </c>
+      <c r="E26" t="n">
+        <v>1303.1</v>
+      </c>
+      <c r="F26" t="n">
+        <v>-8.73</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1418.829956054688</v>
+      </c>
+      <c r="H26" t="n">
+        <v>-0.6200000047683716</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J26" t="n">
+        <v>0.886</v>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="M26" t="n">
+        <v>54.63</v>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>SBIN.NS</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>1007.15</v>
+      </c>
+      <c r="E27" t="n">
+        <v>964.3099999999999</v>
+      </c>
+      <c r="F27" t="n">
+        <v>-4.25</v>
+      </c>
+      <c r="G27" t="n">
+        <v>1069.150024414062</v>
+      </c>
+      <c r="H27" t="n">
+        <v>6.159999847412109</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J27" t="n">
+        <v>0.725</v>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="M27" t="n">
+        <v>58.12</v>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>HINDUNILVR.NS</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>2399.4</v>
+      </c>
+      <c r="E28" t="n">
+        <v>2315.68</v>
+      </c>
+      <c r="F28" t="n">
+        <v>-3.49</v>
+      </c>
+      <c r="G28" t="n">
+        <v>2395.719970703125</v>
+      </c>
+      <c r="H28" t="n">
+        <v>-0.1500000059604645</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="J28" t="n">
+        <v>-0.65</v>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>❌ Strong Avoid</t>
+        </is>
+      </c>
+      <c r="M28" t="n">
+        <v>31.77</v>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>ITC.NS</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>341.25</v>
+      </c>
+      <c r="E29" t="n">
+        <v>384.19</v>
+      </c>
+      <c r="F29" t="n">
+        <v>12.58</v>
+      </c>
+      <c r="G29" t="n">
+        <v>368.2900085449219</v>
+      </c>
+      <c r="H29" t="n">
+        <v>7.920000076293945</v>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J29" t="n">
+        <v>0.586</v>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="M29" t="n">
+        <v>80.59</v>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>LT.NS</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>4157</v>
+      </c>
+      <c r="E30" t="n">
+        <v>3967.89</v>
+      </c>
+      <c r="F30" t="n">
+        <v>-4.55</v>
+      </c>
+      <c r="G30" t="n">
+        <v>3983.93994140625</v>
+      </c>
+      <c r="H30" t="n">
+        <v>-4.159999847412109</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="J30" t="n">
+        <v>-0.511</v>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>❌ Strong Avoid</t>
+        </is>
+      </c>
+      <c r="M30" t="n">
+        <v>32.96</v>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>BAJFINANCE.NS</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>968.8</v>
+      </c>
+      <c r="E31" t="n">
+        <v>1019.91</v>
+      </c>
+      <c r="F31" t="n">
+        <v>5.28</v>
+      </c>
+      <c r="G31" t="n">
+        <v>833.5800170898438</v>
+      </c>
+      <c r="H31" t="n">
+        <v>-13.96000003814697</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="J31" t="n">
+        <v>-0.625</v>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>⚠️ Cautious Buy</t>
+        </is>
+      </c>
+      <c r="M31" t="n">
+        <v>45.41</v>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>BHARTIARTL.NS</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>2084.2</v>
+      </c>
+      <c r="E32" t="n">
+        <v>2234.12</v>
+      </c>
+      <c r="F32" t="n">
+        <v>7.19</v>
+      </c>
+      <c r="G32" t="n">
+        <v>2074.06005859375</v>
+      </c>
+      <c r="H32" t="n">
+        <v>-0.4900000095367432</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J32" t="n">
+        <v>0.735</v>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="M32" t="n">
+        <v>75.48999999999999</v>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>ASIANPAINT.NS</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>2809.4</v>
+      </c>
+      <c r="E33" t="n">
+        <v>2728.76</v>
+      </c>
+      <c r="F33" t="n">
+        <v>-2.87</v>
+      </c>
+      <c r="G33" t="n">
+        <v>2756.72998046875</v>
+      </c>
+      <c r="H33" t="n">
+        <v>-1.870000004768372</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J33" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="M33" t="n">
+        <v>58.69</v>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>AXISBANK.NS</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>1295.5</v>
+      </c>
+      <c r="E34" t="n">
+        <v>1184.46</v>
+      </c>
+      <c r="F34" t="n">
+        <v>-8.57</v>
+      </c>
+      <c r="G34" t="n">
+        <v>1210.300048828125</v>
+      </c>
+      <c r="H34" t="n">
+        <v>-6.579999923706055</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J34" t="n">
+        <v>0.848</v>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="M34" t="n">
+        <v>54.1</v>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>MARUTI.NS</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>16809</v>
+      </c>
+      <c r="E35" t="n">
+        <v>18244.16</v>
+      </c>
+      <c r="F35" t="n">
+        <v>8.539999999999999</v>
+      </c>
+      <c r="G35" t="n">
+        <v>18342.619140625</v>
+      </c>
+      <c r="H35" t="n">
+        <v>9.119999885559082</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J35" t="n">
+        <v>0.727</v>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="M35" t="n">
+        <v>77.34999999999999</v>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>SUNPHARMA.NS</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>1782.6</v>
+      </c>
+      <c r="E36" t="n">
+        <v>1824.95</v>
+      </c>
+      <c r="F36" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1577.099975585938</v>
+      </c>
+      <c r="H36" t="n">
+        <v>-11.52999973297119</v>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J36" t="n">
+        <v>0.751</v>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="M36" t="n">
+        <v>68.58</v>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>WIPRO.NS</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>270.8</v>
+      </c>
+      <c r="E37" t="n">
+        <v>276.72</v>
+      </c>
+      <c r="F37" t="n">
+        <v>2.19</v>
+      </c>
+      <c r="G37" t="n">
+        <v>279.0599975585938</v>
+      </c>
+      <c r="H37" t="n">
+        <v>3.049999952316284</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J37" t="n">
+        <v>0.743</v>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="M37" t="n">
+        <v>68.14</v>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>ULTRACEMCO.NS</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>12184</v>
+      </c>
+      <c r="E38" t="n">
+        <v>11548.94</v>
+      </c>
+      <c r="F38" t="n">
+        <v>-5.21</v>
+      </c>
+      <c r="G38" t="n">
+        <v>12051.4404296875</v>
+      </c>
+      <c r="H38" t="n">
+        <v>-1.090000033378601</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J38" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="M38" t="n">
+        <v>55.18</v>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>NTPC.NS</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>348.85</v>
+      </c>
+      <c r="E39" t="n">
+        <v>325.85</v>
+      </c>
+      <c r="F39" t="n">
+        <v>-6.59</v>
+      </c>
+      <c r="G39" t="n">
+        <v>350.9400024414062</v>
+      </c>
+      <c r="H39" t="n">
+        <v>0.6000000238418579</v>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J39" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="M39" t="n">
+        <v>53.11</v>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>POWERGRID.NS</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>264.1</v>
+      </c>
+      <c r="E40" t="n">
+        <v>257.51</v>
+      </c>
+      <c r="F40" t="n">
+        <v>-2.49</v>
+      </c>
+      <c r="G40" t="n">
+        <v>270.8599853515625</v>
+      </c>
+      <c r="H40" t="n">
+        <v>2.559999942779541</v>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J40" t="n">
+        <v>0.784</v>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="M40" t="n">
+        <v>61.94</v>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>TITAN.NS</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>4273.2</v>
+      </c>
+      <c r="E41" t="n">
+        <v>4019.9</v>
+      </c>
+      <c r="F41" t="n">
+        <v>-5.93</v>
+      </c>
+      <c r="G41" t="n">
+        <v>3679.68994140625</v>
+      </c>
+      <c r="H41" t="n">
+        <v>-13.89000034332275</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J41" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="M41" t="n">
+        <v>55.11</v>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:N11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>Market</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>Stock</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>Current Price</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>Prophet Predicted Price</t>
-        </is>
-      </c>
-      <c r="F1" s="2" t="inlineStr">
-        <is>
-          <t>Prophet Return %</t>
-        </is>
-      </c>
-      <c r="G1" s="2" t="inlineStr">
-        <is>
-          <t>LSTM Predicted Price</t>
-        </is>
-      </c>
-      <c r="H1" s="2" t="inlineStr">
-        <is>
-          <t>LSTM Return %</t>
-        </is>
-      </c>
-      <c r="I1" s="2" t="inlineStr">
-        <is>
-          <t>News Sentiment</t>
-        </is>
-      </c>
-      <c r="J1" s="2" t="inlineStr">
-        <is>
-          <t>News Score</t>
-        </is>
-      </c>
-      <c r="K1" s="2" t="inlineStr">
-        <is>
-          <t>Price Trend</t>
-        </is>
-      </c>
-      <c r="L1" s="2" t="inlineStr">
-        <is>
-          <t>Final Recommendation</t>
-        </is>
-      </c>
-      <c r="M1" s="2" t="inlineStr">
-        <is>
-          <t>Confidence Score %</t>
-        </is>
-      </c>
-      <c r="N1" s="2" t="inlineStr">
-        <is>
-          <t>Last Updated</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2026-01-07</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>BSE</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>RELIANCE.BO</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>1507.7</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1697.95</v>
-      </c>
-      <c r="F2" t="n">
-        <v>12.62</v>
-      </c>
-      <c r="G2" t="n">
-        <v>1486.489990234375</v>
-      </c>
-      <c r="H2" t="n">
-        <v>-1.409999966621399</v>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Negative</t>
-        </is>
-      </c>
-      <c r="J2" t="n">
-        <v>-0.65</v>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>Up</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>⚠️ Cautious Buy</t>
-        </is>
-      </c>
-      <c r="M2" t="n">
-        <v>55.93</v>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>07 Jan 2026, 09:28:05 PM IST</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2026-01-07</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>BSE</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>TCS.BO</t>
-        </is>
-      </c>
-      <c r="D3" t="n">
-        <v>3255.75</v>
-      </c>
-      <c r="E3" t="n">
-        <v>3241.44</v>
-      </c>
-      <c r="F3" t="n">
-        <v>-0.44</v>
-      </c>
-      <c r="G3" t="n">
-        <v>3234.699951171875</v>
-      </c>
-      <c r="H3" t="n">
-        <v>-0.6499999761581421</v>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
-      </c>
-      <c r="J3" t="n">
-        <v>0.796</v>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>Down</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>⚠️ Speculative Buy</t>
-        </is>
-      </c>
-      <c r="M3" t="n">
-        <v>65.26000000000001</v>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>07 Jan 2026, 09:28:05 PM IST</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2026-01-07</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>BSE</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>INFY.BO</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>1611.15</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1651.79</v>
-      </c>
-      <c r="F4" t="n">
-        <v>2.52</v>
-      </c>
-      <c r="G4" t="n">
-        <v>1526.93994140625</v>
-      </c>
-      <c r="H4" t="n">
-        <v>-5.230000019073486</v>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
-      </c>
-      <c r="J4" t="n">
-        <v>0.836</v>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>Up</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>🚀 Strong Buy</t>
-        </is>
-      </c>
-      <c r="M4" t="n">
-        <v>70.5</v>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>07 Jan 2026, 09:28:05 PM IST</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2026-01-07</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>BSE</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>HDFCBANK.BO</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>962.4</v>
-      </c>
-      <c r="E5" t="n">
-        <v>932</v>
-      </c>
-      <c r="F5" t="n">
-        <v>-3.16</v>
-      </c>
-      <c r="G5" t="n">
-        <v>1016.52001953125</v>
-      </c>
-      <c r="H5" t="n">
-        <v>5.619999885559082</v>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Negative</t>
-        </is>
-      </c>
-      <c r="J5" t="n">
-        <v>-0.612</v>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>Down</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>❌ Strong Avoid</t>
-        </is>
-      </c>
-      <c r="M5" t="n">
-        <v>33.02</v>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>07 Jan 2026, 09:28:05 PM IST</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2026-01-07</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>BSE</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>ICICIBANK.BO</t>
-        </is>
-      </c>
-      <c r="D6" t="n">
-        <v>1410.75</v>
-      </c>
-      <c r="E6" t="n">
-        <v>1295.12</v>
-      </c>
-      <c r="F6" t="n">
-        <v>-8.199999999999999</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1444.31005859375</v>
-      </c>
-      <c r="H6" t="n">
-        <v>2.380000114440918</v>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
-      </c>
-      <c r="J6" t="n">
-        <v>0.459</v>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>Down</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>⚠️ Speculative Buy</t>
-        </is>
-      </c>
-      <c r="M6" t="n">
-        <v>46.89</v>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>07 Jan 2026, 09:28:05 PM IST</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2026-01-07</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>BSE</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>SBIN.BO</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>1018.75</v>
-      </c>
-      <c r="E7" t="n">
-        <v>968.42</v>
-      </c>
-      <c r="F7" t="n">
-        <v>-4.94</v>
-      </c>
-      <c r="G7" t="n">
-        <v>1048.050048828125</v>
-      </c>
-      <c r="H7" t="n">
-        <v>2.880000114440918</v>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
-      </c>
-      <c r="J7" t="n">
-        <v>0.527</v>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>Down</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>⚠️ Speculative Buy</t>
-        </is>
-      </c>
-      <c r="M7" t="n">
-        <v>53.13</v>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>07 Jan 2026, 09:28:05 PM IST</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2026-01-07</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>BSE</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>ITC.BO</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>342.45</v>
-      </c>
-      <c r="E8" t="n">
-        <v>378.32</v>
-      </c>
-      <c r="F8" t="n">
-        <v>10.47</v>
-      </c>
-      <c r="G8" t="n">
-        <v>382.989990234375</v>
-      </c>
-      <c r="H8" t="n">
-        <v>11.84000015258789</v>
-      </c>
-      <c r="I8" t="inlineStr">
-        <is>
-          <t>Negative</t>
-        </is>
-      </c>
-      <c r="J8" t="n">
-        <v>-0.751</v>
-      </c>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>Up</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>⚠️ Cautious Buy</t>
-        </is>
-      </c>
-      <c r="M8" t="n">
-        <v>50.69</v>
-      </c>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>07 Jan 2026, 09:28:05 PM IST</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2026-01-07</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>BSE</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>LT.BO</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>4141.3</v>
-      </c>
-      <c r="E9" t="n">
-        <v>3983.32</v>
-      </c>
-      <c r="F9" t="n">
-        <v>-3.81</v>
-      </c>
-      <c r="G9" t="n">
-        <v>4153.06005859375</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.2800000011920929</v>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
-      </c>
-      <c r="J9" t="n">
-        <v>0.465</v>
-      </c>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>Down</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>⚠️ Speculative Buy</t>
-        </is>
-      </c>
-      <c r="M9" t="n">
-        <v>53.58</v>
-      </c>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>07 Jan 2026, 09:28:05 PM IST</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2026-01-07</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>BSE</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>AXISBANK.BO</t>
-        </is>
-      </c>
-      <c r="D10" t="n">
-        <v>1293.6</v>
-      </c>
-      <c r="E10" t="n">
-        <v>1200.74</v>
-      </c>
-      <c r="F10" t="n">
-        <v>-7.18</v>
-      </c>
-      <c r="G10" t="n">
-        <v>1261.22998046875</v>
-      </c>
-      <c r="H10" t="n">
-        <v>-2.5</v>
-      </c>
-      <c r="I10" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
-      </c>
-      <c r="J10" t="n">
-        <v>0.848</v>
-      </c>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>Down</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>⚠️ Speculative Buy</t>
-        </is>
-      </c>
-      <c r="M10" t="n">
-        <v>56.19</v>
-      </c>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>07 Jan 2026, 09:28:05 PM IST</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2026-01-07</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>BSE</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>MARUTI.BO</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>17294.95</v>
-      </c>
-      <c r="E11" t="n">
-        <v>18383.19</v>
-      </c>
-      <c r="F11" t="n">
-        <v>6.29</v>
-      </c>
-      <c r="G11" t="n">
-        <v>17491.669921875</v>
-      </c>
-      <c r="H11" t="n">
-        <v>1.139999985694885</v>
-      </c>
-      <c r="I11" t="inlineStr">
-        <is>
-          <t>Positive</t>
-        </is>
-      </c>
-      <c r="J11" t="n">
-        <v>0.681</v>
-      </c>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>Up</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>🚀 Strong Buy</t>
-        </is>
-      </c>
-      <c r="M11" t="n">
-        <v>73.06</v>
-      </c>
-      <c r="N11" t="inlineStr">
-        <is>
-          <t>07 Jan 2026, 09:28:05 PM IST</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2462,6 +2951,1257 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>RELIANCE.BO</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>1507.7</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1697.95</v>
+      </c>
+      <c r="F2" t="n">
+        <v>12.62</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1486.489990234375</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-1.409999966621399</v>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="J2" t="n">
+        <v>-0.65</v>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>⚠️ Cautious Buy</t>
+        </is>
+      </c>
+      <c r="M2" t="n">
+        <v>55.93</v>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>07 Jan 2026, 09:28:05 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>TCS.BO</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>3255.75</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3241.44</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-0.44</v>
+      </c>
+      <c r="G3" t="n">
+        <v>3234.699951171875</v>
+      </c>
+      <c r="H3" t="n">
+        <v>-0.6499999761581421</v>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J3" t="n">
+        <v>0.796</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="M3" t="n">
+        <v>65.26000000000001</v>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>07 Jan 2026, 09:28:05 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>INFY.BO</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>1611.15</v>
+      </c>
+      <c r="E4" t="n">
+        <v>1651.79</v>
+      </c>
+      <c r="F4" t="n">
+        <v>2.52</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1526.93994140625</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-5.230000019073486</v>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J4" t="n">
+        <v>0.836</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="M4" t="n">
+        <v>70.5</v>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>07 Jan 2026, 09:28:05 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>HDFCBANK.BO</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>962.4</v>
+      </c>
+      <c r="E5" t="n">
+        <v>932</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-3.16</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1016.52001953125</v>
+      </c>
+      <c r="H5" t="n">
+        <v>5.619999885559082</v>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="J5" t="n">
+        <v>-0.612</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>❌ Strong Avoid</t>
+        </is>
+      </c>
+      <c r="M5" t="n">
+        <v>33.02</v>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>07 Jan 2026, 09:28:05 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>ICICIBANK.BO</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>1410.75</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1295.12</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-8.199999999999999</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1444.31005859375</v>
+      </c>
+      <c r="H6" t="n">
+        <v>2.380000114440918</v>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J6" t="n">
+        <v>0.459</v>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="M6" t="n">
+        <v>46.89</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>07 Jan 2026, 09:28:05 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>SBIN.BO</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>1018.75</v>
+      </c>
+      <c r="E7" t="n">
+        <v>968.42</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-4.94</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1048.050048828125</v>
+      </c>
+      <c r="H7" t="n">
+        <v>2.880000114440918</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J7" t="n">
+        <v>0.527</v>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="M7" t="n">
+        <v>53.13</v>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>07 Jan 2026, 09:28:05 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>ITC.BO</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>342.45</v>
+      </c>
+      <c r="E8" t="n">
+        <v>378.32</v>
+      </c>
+      <c r="F8" t="n">
+        <v>10.47</v>
+      </c>
+      <c r="G8" t="n">
+        <v>382.989990234375</v>
+      </c>
+      <c r="H8" t="n">
+        <v>11.84000015258789</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="J8" t="n">
+        <v>-0.751</v>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>⚠️ Cautious Buy</t>
+        </is>
+      </c>
+      <c r="M8" t="n">
+        <v>50.69</v>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>07 Jan 2026, 09:28:05 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>LT.BO</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>4141.3</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3983.32</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-3.81</v>
+      </c>
+      <c r="G9" t="n">
+        <v>4153.06005859375</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.2800000011920929</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J9" t="n">
+        <v>0.465</v>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="M9" t="n">
+        <v>53.58</v>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>07 Jan 2026, 09:28:05 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>AXISBANK.BO</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>1293.6</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1200.74</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-7.18</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1261.22998046875</v>
+      </c>
+      <c r="H10" t="n">
+        <v>-2.5</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J10" t="n">
+        <v>0.848</v>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="M10" t="n">
+        <v>56.19</v>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>07 Jan 2026, 09:28:05 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>MARUTI.BO</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>17294.95</v>
+      </c>
+      <c r="E11" t="n">
+        <v>18383.19</v>
+      </c>
+      <c r="F11" t="n">
+        <v>6.29</v>
+      </c>
+      <c r="G11" t="n">
+        <v>17491.669921875</v>
+      </c>
+      <c r="H11" t="n">
+        <v>1.139999985694885</v>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J11" t="n">
+        <v>0.681</v>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="M11" t="n">
+        <v>73.06</v>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>07 Jan 2026, 09:28:05 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>RELIANCE.BO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>1504.1</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1687.45</v>
+      </c>
+      <c r="F12" t="n">
+        <v>12.19</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1455.219970703125</v>
+      </c>
+      <c r="H12" t="n">
+        <v>-3.25</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="J12" t="n">
+        <v>-0.784</v>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>⚠️ Cautious Buy</t>
+        </is>
+      </c>
+      <c r="M12" t="n">
+        <v>52.61</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>TCS.BO</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>3294.45</v>
+      </c>
+      <c r="E13" t="n">
+        <v>3261.11</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-1.01</v>
+      </c>
+      <c r="G13" t="n">
+        <v>3207.489990234375</v>
+      </c>
+      <c r="H13" t="n">
+        <v>-2.640000104904175</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J13" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="M13" t="n">
+        <v>61.48</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>INFY.BO</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>1638.9</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1650.72</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1835.510009765625</v>
+      </c>
+      <c r="H14" t="n">
+        <v>12</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="J14" t="n">
+        <v>-0.477</v>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>⚠️ Cautious Buy</t>
+        </is>
+      </c>
+      <c r="M14" t="n">
+        <v>41.54</v>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>HDFCBANK.BO</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>949.15</v>
+      </c>
+      <c r="E15" t="n">
+        <v>930.75</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-1.94</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1008.77001953125</v>
+      </c>
+      <c r="H15" t="n">
+        <v>6.28000020980835</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="J15" t="n">
+        <v>-0.65</v>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>❌ Strong Avoid</t>
+        </is>
+      </c>
+      <c r="M15" t="n">
+        <v>34.09</v>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>ICICIBANK.BO</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>1428.45</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1305.62</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-8.6</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1327.910034179688</v>
+      </c>
+      <c r="H16" t="n">
+        <v>-7.039999961853027</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J16" t="n">
+        <v>0.886</v>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="M16" t="n">
+        <v>54.82</v>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>SBIN.BO</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>1007.1</v>
+      </c>
+      <c r="E17" t="n">
+        <v>970.85</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-3.6</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1059.410034179688</v>
+      </c>
+      <c r="H17" t="n">
+        <v>5.190000057220459</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J17" t="n">
+        <v>0.725</v>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="M17" t="n">
+        <v>59.1</v>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>ITC.BO</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>341.35</v>
+      </c>
+      <c r="E18" t="n">
+        <v>378.12</v>
+      </c>
+      <c r="F18" t="n">
+        <v>10.77</v>
+      </c>
+      <c r="G18" t="n">
+        <v>383.4700012207031</v>
+      </c>
+      <c r="H18" t="n">
+        <v>12.34000015258789</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J18" t="n">
+        <v>0.586</v>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="M18" t="n">
+        <v>77.88</v>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>LT.BO</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>4167.8</v>
+      </c>
+      <c r="E19" t="n">
+        <v>3976.72</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-4.58</v>
+      </c>
+      <c r="G19" t="n">
+        <v>4011.580078125</v>
+      </c>
+      <c r="H19" t="n">
+        <v>-3.75</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="J19" t="n">
+        <v>-0.511</v>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>❌ Strong Avoid</t>
+        </is>
+      </c>
+      <c r="M19" t="n">
+        <v>32.9</v>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>AXISBANK.BO</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>1295.85</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1204.16</v>
+      </c>
+      <c r="F20" t="n">
+        <v>-7.08</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1133</v>
+      </c>
+      <c r="H20" t="n">
+        <v>-12.56999969482422</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J20" t="n">
+        <v>0.848</v>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="M20" t="n">
+        <v>56.35</v>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>MARUTI.BO</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>16803.8</v>
+      </c>
+      <c r="E21" t="n">
+        <v>18344.55</v>
+      </c>
+      <c r="F21" t="n">
+        <v>9.17</v>
+      </c>
+      <c r="G21" t="n">
+        <v>18439.380859375</v>
+      </c>
+      <c r="H21" t="n">
+        <v>9.729999542236328</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J21" t="n">
+        <v>0.727</v>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="M21" t="n">
+        <v>78.29000000000001</v>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:N41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Market</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Stock</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Current Price</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Prophet Predicted Price</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Prophet Return %</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>LSTM Predicted Price</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>LSTM Return %</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>News Sentiment</t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>News Score</t>
+        </is>
+      </c>
+      <c r="K1" s="2" t="inlineStr">
+        <is>
+          <t>Price Trend</t>
+        </is>
+      </c>
+      <c r="L1" s="2" t="inlineStr">
+        <is>
+          <t>Final Recommendation</t>
+        </is>
+      </c>
+      <c r="M1" s="2" t="inlineStr">
+        <is>
+          <t>Confidence Score %</t>
+        </is>
+      </c>
+      <c r="N1" s="2" t="inlineStr">
+        <is>
+          <t>Last Updated</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2026-01-07</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>NYSE</t>
         </is>
       </c>
@@ -3611,6 +5351,1166 @@
       <c r="N21" t="inlineStr">
         <is>
           <t>07 Jan 2026, 09:28:05 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>260.33</v>
+      </c>
+      <c r="E22" t="n">
+        <v>287.68</v>
+      </c>
+      <c r="F22" t="n">
+        <v>10.5</v>
+      </c>
+      <c r="G22" t="n">
+        <v>280</v>
+      </c>
+      <c r="H22" t="n">
+        <v>7.559999942779541</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J22" t="n">
+        <v>0.784</v>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="M22" t="n">
+        <v>81.44</v>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>MSFT</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>483.47</v>
+      </c>
+      <c r="E23" t="n">
+        <v>480.8</v>
+      </c>
+      <c r="F23" t="n">
+        <v>-0.55</v>
+      </c>
+      <c r="G23" t="n">
+        <v>478.5299987792969</v>
+      </c>
+      <c r="H23" t="n">
+        <v>-1.019999980926514</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="J23" t="n">
+        <v>0</v>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>🔻 Avoid</t>
+        </is>
+      </c>
+      <c r="M23" t="n">
+        <v>49.17</v>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>GOOGL</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>321.98</v>
+      </c>
+      <c r="E24" t="n">
+        <v>357.92</v>
+      </c>
+      <c r="F24" t="n">
+        <v>11.16</v>
+      </c>
+      <c r="G24" t="n">
+        <v>326.6000061035156</v>
+      </c>
+      <c r="H24" t="n">
+        <v>1.429999947547913</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J24" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="M24" t="n">
+        <v>79.73999999999999</v>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>241.56</v>
+      </c>
+      <c r="E25" t="n">
+        <v>251.27</v>
+      </c>
+      <c r="F25" t="n">
+        <v>4.02</v>
+      </c>
+      <c r="G25" t="n">
+        <v>225.9900054931641</v>
+      </c>
+      <c r="H25" t="n">
+        <v>-6.449999809265137</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="J25" t="n">
+        <v>0.178</v>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>🟢 Buy</t>
+        </is>
+      </c>
+      <c r="M25" t="n">
+        <v>59.59</v>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>META</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>648.6900000000001</v>
+      </c>
+      <c r="E26" t="n">
+        <v>718.83</v>
+      </c>
+      <c r="F26" t="n">
+        <v>10.81</v>
+      </c>
+      <c r="G26" t="n">
+        <v>673.1199951171875</v>
+      </c>
+      <c r="H26" t="n">
+        <v>3.769999980926514</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J26" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="M26" t="n">
+        <v>79.22</v>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>431.41</v>
+      </c>
+      <c r="E27" t="n">
+        <v>457.8</v>
+      </c>
+      <c r="F27" t="n">
+        <v>6.12</v>
+      </c>
+      <c r="G27" t="n">
+        <v>423.2099914550781</v>
+      </c>
+      <c r="H27" t="n">
+        <v>-1.899999976158142</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="J27" t="n">
+        <v>-0.65</v>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>⚠️ Cautious Buy</t>
+        </is>
+      </c>
+      <c r="M27" t="n">
+        <v>46.18</v>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>189.11</v>
+      </c>
+      <c r="E28" t="n">
+        <v>202.55</v>
+      </c>
+      <c r="F28" t="n">
+        <v>7.11</v>
+      </c>
+      <c r="G28" t="n">
+        <v>206.8800048828125</v>
+      </c>
+      <c r="H28" t="n">
+        <v>9.399999618530273</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J28" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="M28" t="n">
+        <v>73.66</v>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>JPM</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>326.99</v>
+      </c>
+      <c r="E29" t="n">
+        <v>342.61</v>
+      </c>
+      <c r="F29" t="n">
+        <v>4.78</v>
+      </c>
+      <c r="G29" t="n">
+        <v>388.3200073242188</v>
+      </c>
+      <c r="H29" t="n">
+        <v>18.76000022888184</v>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J29" t="n">
+        <v>0.511</v>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="M29" t="n">
+        <v>67.38</v>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>355.88</v>
+      </c>
+      <c r="E30" t="n">
+        <v>358.53</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="G30" t="n">
+        <v>352.1300048828125</v>
+      </c>
+      <c r="H30" t="n">
+        <v>-1.049999952316284</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J30" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="M30" t="n">
+        <v>64.31999999999999</v>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>JNJ</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
+        <v>207.49</v>
+      </c>
+      <c r="E31" t="n">
+        <v>219.37</v>
+      </c>
+      <c r="F31" t="n">
+        <v>5.73</v>
+      </c>
+      <c r="G31" t="n">
+        <v>231.2700042724609</v>
+      </c>
+      <c r="H31" t="n">
+        <v>11.46000003814697</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J31" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="M31" t="n">
+        <v>71.79000000000001</v>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>WMT</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>112.72</v>
+      </c>
+      <c r="E32" t="n">
+        <v>116.33</v>
+      </c>
+      <c r="F32" t="n">
+        <v>3.21</v>
+      </c>
+      <c r="G32" t="n">
+        <v>95.98000335693359</v>
+      </c>
+      <c r="H32" t="n">
+        <v>-14.85000038146973</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J32" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="M32" t="n">
+        <v>68.01000000000001</v>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>PG</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>138.04</v>
+      </c>
+      <c r="E33" t="n">
+        <v>143.77</v>
+      </c>
+      <c r="F33" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="G33" t="n">
+        <v>148.1000061035156</v>
+      </c>
+      <c r="H33" t="n">
+        <v>7.289999961853027</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J33" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="M33" t="n">
+        <v>69.42</v>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>MA</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
+        <v>579.92</v>
+      </c>
+      <c r="E34" t="n">
+        <v>583.39</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="G34" t="n">
+        <v>580.22998046875</v>
+      </c>
+      <c r="H34" t="n">
+        <v>0.05000000074505806</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J34" t="n">
+        <v>0.572</v>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="M34" t="n">
+        <v>62.34</v>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>UNH</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>341.7</v>
+      </c>
+      <c r="E35" t="n">
+        <v>302.73</v>
+      </c>
+      <c r="F35" t="n">
+        <v>-11.4</v>
+      </c>
+      <c r="G35" t="n">
+        <v>315.4700012207031</v>
+      </c>
+      <c r="H35" t="n">
+        <v>-7.679999828338623</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J35" t="n">
+        <v>0.751</v>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="M35" t="n">
+        <v>47.91</v>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>HD</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>349.06</v>
+      </c>
+      <c r="E36" t="n">
+        <v>343.07</v>
+      </c>
+      <c r="F36" t="n">
+        <v>-1.72</v>
+      </c>
+      <c r="G36" t="n">
+        <v>336.510009765625</v>
+      </c>
+      <c r="H36" t="n">
+        <v>-3.599999904632568</v>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J36" t="n">
+        <v>0.572</v>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="M36" t="n">
+        <v>58.86</v>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>BAC</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>55.64</v>
+      </c>
+      <c r="E37" t="n">
+        <v>57.4</v>
+      </c>
+      <c r="F37" t="n">
+        <v>3.16</v>
+      </c>
+      <c r="G37" t="n">
+        <v>62.2599983215332</v>
+      </c>
+      <c r="H37" t="n">
+        <v>11.89000034332275</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J37" t="n">
+        <v>0.827</v>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="M37" t="n">
+        <v>71.27</v>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>XOM</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>118.49</v>
+      </c>
+      <c r="E38" t="n">
+        <v>119.85</v>
+      </c>
+      <c r="F38" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="G38" t="n">
+        <v>108.3199996948242</v>
+      </c>
+      <c r="H38" t="n">
+        <v>-8.579999923706055</v>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J38" t="n">
+        <v>0.5570000000000001</v>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="M38" t="n">
+        <v>62.87</v>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>AVGO</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>343.5</v>
+      </c>
+      <c r="E39" t="n">
+        <v>421.81</v>
+      </c>
+      <c r="F39" t="n">
+        <v>22.8</v>
+      </c>
+      <c r="G39" t="n">
+        <v>316.9200134277344</v>
+      </c>
+      <c r="H39" t="n">
+        <v>-7.739999771118164</v>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J39" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="M39" t="n">
+        <v>93.2</v>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>COST</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>882.58</v>
+      </c>
+      <c r="E40" t="n">
+        <v>904.61</v>
+      </c>
+      <c r="F40" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="G40" t="n">
+        <v>969.1699829101562</v>
+      </c>
+      <c r="H40" t="n">
+        <v>9.810000419616699</v>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J40" t="n">
+        <v>0.832</v>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="M40" t="n">
+        <v>70.38</v>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2026-01-08</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>PEP</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>137.01</v>
+      </c>
+      <c r="E41" t="n">
+        <v>147.77</v>
+      </c>
+      <c r="F41" t="n">
+        <v>7.86</v>
+      </c>
+      <c r="G41" t="n">
+        <v>152.0500030517578</v>
+      </c>
+      <c r="H41" t="n">
+        <v>10.97999954223633</v>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="J41" t="n">
+        <v>0.758</v>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="M41" t="n">
+        <v>76.94</v>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>08 Jan 2026, 06:53:43 PM IST</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Daily StockIQ Insights update (2026-01-10)
</commit_message>
<xml_diff>
--- a/Daily_StockIQ_Insights.xlsx
+++ b/Daily_StockIQ_Insights.xlsx
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O41"/>
+  <dimension ref="A1:O61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3329,6 +3329,1266 @@
       <c r="O41" t="inlineStr">
         <is>
           <t>09 Jan 2026, 06:52:05 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>RELIANCE.NS</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Reliance Industries Limited</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>1475.3</v>
+      </c>
+      <c r="F42" t="n">
+        <v>1674.01</v>
+      </c>
+      <c r="G42" t="n">
+        <v>13.47</v>
+      </c>
+      <c r="H42" t="n">
+        <v>1530.449951171875</v>
+      </c>
+      <c r="I42" t="n">
+        <v>3.740000009536743</v>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K42" t="n">
+        <v>0.883</v>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N42" t="n">
+        <v>87.86</v>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>TCS.NS</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Tata Consultancy Services Limited</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>3207.8</v>
+      </c>
+      <c r="F43" t="n">
+        <v>3269.45</v>
+      </c>
+      <c r="G43" t="n">
+        <v>1.92</v>
+      </c>
+      <c r="H43" t="n">
+        <v>3231.47998046875</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0.7400000095367432</v>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="K43" t="n">
+        <v>-0.743</v>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>⚠️ Cautious Buy</t>
+        </is>
+      </c>
+      <c r="N43" t="n">
+        <v>38.02</v>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>INFY.NS</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Infosys Limited</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>1614.1</v>
+      </c>
+      <c r="F44" t="n">
+        <v>1654.73</v>
+      </c>
+      <c r="G44" t="n">
+        <v>2.52</v>
+      </c>
+      <c r="H44" t="n">
+        <v>1361.930053710938</v>
+      </c>
+      <c r="I44" t="n">
+        <v>-15.61999988555908</v>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K44" t="n">
+        <v>0.718</v>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N44" t="n">
+        <v>68.14</v>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>HDFCBANK.NS</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>HDFC Bank Limited</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>939</v>
+      </c>
+      <c r="F45" t="n">
+        <v>921.91</v>
+      </c>
+      <c r="G45" t="n">
+        <v>-1.82</v>
+      </c>
+      <c r="H45" t="n">
+        <v>899.02001953125</v>
+      </c>
+      <c r="I45" t="n">
+        <v>-4.260000228881836</v>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K45" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N45" t="n">
+        <v>60.27</v>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>ICICIBANK.NS</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>ICICI Bank Limited</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>1404.3</v>
+      </c>
+      <c r="F46" t="n">
+        <v>1323.79</v>
+      </c>
+      <c r="G46" t="n">
+        <v>-5.73</v>
+      </c>
+      <c r="H46" t="n">
+        <v>1414.56005859375</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0.7300000190734863</v>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="K46" t="n">
+        <v>-0.65</v>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>❌ Strong Avoid</t>
+        </is>
+      </c>
+      <c r="N46" t="n">
+        <v>28.4</v>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>SBIN.NS</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>State Bank of India</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>1000.5</v>
+      </c>
+      <c r="F47" t="n">
+        <v>978.02</v>
+      </c>
+      <c r="G47" t="n">
+        <v>-2.25</v>
+      </c>
+      <c r="H47" t="n">
+        <v>886.8200073242188</v>
+      </c>
+      <c r="I47" t="n">
+        <v>-11.35999965667725</v>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K47" t="n">
+        <v>0.494</v>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N47" t="n">
+        <v>56.51</v>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>HINDUNILVR.NS</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Hindustan Unilever Limited</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>2372.6</v>
+      </c>
+      <c r="F48" t="n">
+        <v>2324.41</v>
+      </c>
+      <c r="G48" t="n">
+        <v>-2.03</v>
+      </c>
+      <c r="H48" t="n">
+        <v>2289.010009765625</v>
+      </c>
+      <c r="I48" t="n">
+        <v>-3.519999980926514</v>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="K48" t="n">
+        <v>-0.65</v>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>❌ Strong Avoid</t>
+        </is>
+      </c>
+      <c r="N48" t="n">
+        <v>33.95</v>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>ITC.NS</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>ITC Limited</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>337.15</v>
+      </c>
+      <c r="F49" t="n">
+        <v>371.7</v>
+      </c>
+      <c r="G49" t="n">
+        <v>10.25</v>
+      </c>
+      <c r="H49" t="n">
+        <v>385.760009765625</v>
+      </c>
+      <c r="I49" t="n">
+        <v>14.42000007629395</v>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K49" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N49" t="n">
+        <v>78.37</v>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>LT.NS</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Larsen &amp; Toubro Limited</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>4025.2</v>
+      </c>
+      <c r="F50" t="n">
+        <v>3958.82</v>
+      </c>
+      <c r="G50" t="n">
+        <v>-1.65</v>
+      </c>
+      <c r="H50" t="n">
+        <v>3773.389892578125</v>
+      </c>
+      <c r="I50" t="n">
+        <v>-6.260000228881836</v>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K50" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N50" t="n">
+        <v>54.33</v>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>BAJFINANCE.NS</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Bajaj Finance Limited</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>959.6</v>
+      </c>
+      <c r="F51" t="n">
+        <v>1024.05</v>
+      </c>
+      <c r="G51" t="n">
+        <v>6.72</v>
+      </c>
+      <c r="H51" t="n">
+        <v>1192.160034179688</v>
+      </c>
+      <c r="I51" t="n">
+        <v>24.22999954223633</v>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K51" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N51" t="n">
+        <v>73.06999999999999</v>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>BHARTIARTL.NS</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Bharti Airtel Limited</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>2027.1</v>
+      </c>
+      <c r="F52" t="n">
+        <v>2216.93</v>
+      </c>
+      <c r="G52" t="n">
+        <v>9.359999999999999</v>
+      </c>
+      <c r="H52" t="n">
+        <v>2335.3798828125</v>
+      </c>
+      <c r="I52" t="n">
+        <v>15.21000003814697</v>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K52" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N52" t="n">
+        <v>76.55</v>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>ASIANPAINT.NS</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Asian Paints Limited</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>2825.5</v>
+      </c>
+      <c r="F53" t="n">
+        <v>2740.27</v>
+      </c>
+      <c r="G53" t="n">
+        <v>-3.02</v>
+      </c>
+      <c r="H53" t="n">
+        <v>3054.2900390625</v>
+      </c>
+      <c r="I53" t="n">
+        <v>8.100000381469727</v>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K53" t="n">
+        <v>0.718</v>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N53" t="n">
+        <v>59.84</v>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>AXISBANK.NS</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Axis Bank Limited</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>1272</v>
+      </c>
+      <c r="F54" t="n">
+        <v>1211.49</v>
+      </c>
+      <c r="G54" t="n">
+        <v>-4.76</v>
+      </c>
+      <c r="H54" t="n">
+        <v>1145.339965820312</v>
+      </c>
+      <c r="I54" t="n">
+        <v>-9.960000038146973</v>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K54" t="n">
+        <v>0.852</v>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N54" t="n">
+        <v>59.9</v>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>MARUTI.NS</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Maruti Suzuki India Limited</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>16501</v>
+      </c>
+      <c r="F55" t="n">
+        <v>18406.29</v>
+      </c>
+      <c r="G55" t="n">
+        <v>11.55</v>
+      </c>
+      <c r="H55" t="n">
+        <v>15534.6298828125</v>
+      </c>
+      <c r="I55" t="n">
+        <v>-5.860000133514404</v>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K55" t="n">
+        <v>0.727</v>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N55" t="n">
+        <v>81.86</v>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>SUNPHARMA.NS</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Sun Pharmaceutical Industries Limited</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>1729.9</v>
+      </c>
+      <c r="F56" t="n">
+        <v>1817.88</v>
+      </c>
+      <c r="G56" t="n">
+        <v>5.09</v>
+      </c>
+      <c r="H56" t="n">
+        <v>1659.069946289062</v>
+      </c>
+      <c r="I56" t="n">
+        <v>-4.090000152587891</v>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K56" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N56" t="n">
+        <v>70.63</v>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>WIPRO.NS</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Wipro Limited</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>261.95</v>
+      </c>
+      <c r="F57" t="n">
+        <v>278.61</v>
+      </c>
+      <c r="G57" t="n">
+        <v>6.36</v>
+      </c>
+      <c r="H57" t="n">
+        <v>230.2400054931641</v>
+      </c>
+      <c r="I57" t="n">
+        <v>-12.10999965667725</v>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K57" t="n">
+        <v>0.743</v>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N57" t="n">
+        <v>74.40000000000001</v>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>ULTRACEMCO.NS</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>UltraTech Cement Limited</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>11937</v>
+      </c>
+      <c r="F58" t="n">
+        <v>11598.83</v>
+      </c>
+      <c r="G58" t="n">
+        <v>-2.83</v>
+      </c>
+      <c r="H58" t="n">
+        <v>11242.58984375</v>
+      </c>
+      <c r="I58" t="n">
+        <v>-5.820000171661377</v>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K58" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N58" t="n">
+        <v>58.75</v>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>NTPC.NS</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>NTPC Limited</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>336</v>
+      </c>
+      <c r="F59" t="n">
+        <v>327.07</v>
+      </c>
+      <c r="G59" t="n">
+        <v>-2.66</v>
+      </c>
+      <c r="H59" t="n">
+        <v>407.0400085449219</v>
+      </c>
+      <c r="I59" t="n">
+        <v>21.13999938964844</v>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K59" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N59" t="n">
+        <v>59.02</v>
+      </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>POWERGRID.NS</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Power Grid Corporation of India Limited</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>258</v>
+      </c>
+      <c r="F60" t="n">
+        <v>256.21</v>
+      </c>
+      <c r="G60" t="n">
+        <v>-0.6899999999999999</v>
+      </c>
+      <c r="H60" t="n">
+        <v>226.4499969482422</v>
+      </c>
+      <c r="I60" t="n">
+        <v>-12.22999954223633</v>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K60" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N60" t="n">
+        <v>62.96</v>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>TITAN.NS</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Titan Company Limited</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>4201.8</v>
+      </c>
+      <c r="F61" t="n">
+        <v>4110.33</v>
+      </c>
+      <c r="G61" t="n">
+        <v>-2.18</v>
+      </c>
+      <c r="H61" t="n">
+        <v>3404.5</v>
+      </c>
+      <c r="I61" t="n">
+        <v>-18.97999954223633</v>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K61" t="n">
+        <v>0.765</v>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N61" t="n">
+        <v>62.03</v>
+      </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
         </is>
       </c>
     </row>
@@ -3343,7 +4603,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4825,6 +6085,636 @@
       <c r="O21" t="inlineStr">
         <is>
           <t>09 Jan 2026, 06:52:05 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>RELIANCE.BO</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Reliance Industries Limited</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>1475.3</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1678.94</v>
+      </c>
+      <c r="G22" t="n">
+        <v>13.8</v>
+      </c>
+      <c r="H22" t="n">
+        <v>1627.2099609375</v>
+      </c>
+      <c r="I22" t="n">
+        <v>10.30000019073486</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K22" t="n">
+        <v>0.883</v>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N22" t="n">
+        <v>88.36</v>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>TCS.BO</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Tata Consultancy Services Limited</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>3208</v>
+      </c>
+      <c r="F23" t="n">
+        <v>3261.2</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1.66</v>
+      </c>
+      <c r="H23" t="n">
+        <v>3214.10009765625</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.1899999976158142</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="K23" t="n">
+        <v>-0.743</v>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>⚠️ Cautious Buy</t>
+        </is>
+      </c>
+      <c r="N23" t="n">
+        <v>37.63</v>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>INFY.BO</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Infosys Limited</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>1614.75</v>
+      </c>
+      <c r="F24" t="n">
+        <v>1669.38</v>
+      </c>
+      <c r="G24" t="n">
+        <v>3.38</v>
+      </c>
+      <c r="H24" t="n">
+        <v>1557.02001953125</v>
+      </c>
+      <c r="I24" t="n">
+        <v>-3.569999933242798</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K24" t="n">
+        <v>0.718</v>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N24" t="n">
+        <v>69.44</v>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>HDFCBANK.BO</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>HDFC Bank Limited</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>938.7</v>
+      </c>
+      <c r="F25" t="n">
+        <v>924.79</v>
+      </c>
+      <c r="G25" t="n">
+        <v>-1.48</v>
+      </c>
+      <c r="H25" t="n">
+        <v>924.7999877929688</v>
+      </c>
+      <c r="I25" t="n">
+        <v>-1.480000019073486</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K25" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N25" t="n">
+        <v>60.78</v>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>ICICIBANK.BO</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>ICICI Bank Limited</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>1403.55</v>
+      </c>
+      <c r="F26" t="n">
+        <v>1330.11</v>
+      </c>
+      <c r="G26" t="n">
+        <v>-5.23</v>
+      </c>
+      <c r="H26" t="n">
+        <v>1419.969970703125</v>
+      </c>
+      <c r="I26" t="n">
+        <v>1.169999957084656</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="K26" t="n">
+        <v>-0.65</v>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>❌ Strong Avoid</t>
+        </is>
+      </c>
+      <c r="N26" t="n">
+        <v>29.15</v>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>SBIN.BO</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>State Bank of India</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F27" t="n">
+        <v>982.23</v>
+      </c>
+      <c r="G27" t="n">
+        <v>-1.78</v>
+      </c>
+      <c r="H27" t="n">
+        <v>882.0700073242188</v>
+      </c>
+      <c r="I27" t="n">
+        <v>-11.78999996185303</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K27" t="n">
+        <v>0.494</v>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N27" t="n">
+        <v>57.21</v>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>ITC.BO</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>ITC Limited</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>337.1</v>
+      </c>
+      <c r="F28" t="n">
+        <v>370.55</v>
+      </c>
+      <c r="G28" t="n">
+        <v>9.92</v>
+      </c>
+      <c r="H28" t="n">
+        <v>395.0599975585938</v>
+      </c>
+      <c r="I28" t="n">
+        <v>17.19000053405762</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K28" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N28" t="n">
+        <v>77.89</v>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>LT.BO</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Larsen &amp; Toubro Limited</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>4026.75</v>
+      </c>
+      <c r="F29" t="n">
+        <v>3963.48</v>
+      </c>
+      <c r="G29" t="n">
+        <v>-1.57</v>
+      </c>
+      <c r="H29" t="n">
+        <v>3647.5</v>
+      </c>
+      <c r="I29" t="n">
+        <v>-9.420000076293945</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K29" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N29" t="n">
+        <v>54.44</v>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>AXISBANK.BO</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Axis Bank Limited</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>1271.95</v>
+      </c>
+      <c r="F30" t="n">
+        <v>1217.31</v>
+      </c>
+      <c r="G30" t="n">
+        <v>-4.3</v>
+      </c>
+      <c r="H30" t="n">
+        <v>1272.739990234375</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0.05999999865889549</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K30" t="n">
+        <v>0.852</v>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N30" t="n">
+        <v>60.6</v>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>MARUTI.BO</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Maruti Suzuki India Limited</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>16501</v>
+      </c>
+      <c r="F31" t="n">
+        <v>18546.53</v>
+      </c>
+      <c r="G31" t="n">
+        <v>12.4</v>
+      </c>
+      <c r="H31" t="n">
+        <v>19064.94921875</v>
+      </c>
+      <c r="I31" t="n">
+        <v>15.53999996185303</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K31" t="n">
+        <v>0.727</v>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N31" t="n">
+        <v>83.13</v>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
         </is>
       </c>
     </row>
@@ -4839,7 +6729,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O41"/>
+  <dimension ref="A1:O61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7724,6 +9614,1266 @@
         </is>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Apple Inc.</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>259.37</v>
+      </c>
+      <c r="F42" t="n">
+        <v>287.55</v>
+      </c>
+      <c r="G42" t="n">
+        <v>10.86</v>
+      </c>
+      <c r="H42" t="n">
+        <v>272</v>
+      </c>
+      <c r="I42" t="n">
+        <v>4.869999885559082</v>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="K42" t="n">
+        <v>-0.65</v>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>⚠️ Cautious Buy</t>
+        </is>
+      </c>
+      <c r="N42" t="n">
+        <v>53.29</v>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>MSFT</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Microsoft Corporation</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>479.28</v>
+      </c>
+      <c r="F43" t="n">
+        <v>480.27</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="H43" t="n">
+        <v>514.2999877929688</v>
+      </c>
+      <c r="I43" t="n">
+        <v>7.309999942779541</v>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K43" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N43" t="n">
+        <v>63.31</v>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>GOOGL</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Alphabet Inc.</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>328.57</v>
+      </c>
+      <c r="F44" t="n">
+        <v>358.78</v>
+      </c>
+      <c r="G44" t="n">
+        <v>9.19</v>
+      </c>
+      <c r="H44" t="n">
+        <v>259.7699890136719</v>
+      </c>
+      <c r="I44" t="n">
+        <v>-20.94000053405762</v>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K44" t="n">
+        <v>0.402</v>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N44" t="n">
+        <v>71.83</v>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Amazon.com, Inc.</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>247.38</v>
+      </c>
+      <c r="F45" t="n">
+        <v>251.23</v>
+      </c>
+      <c r="G45" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="H45" t="n">
+        <v>201.1100006103516</v>
+      </c>
+      <c r="I45" t="n">
+        <v>-18.70000076293945</v>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K45" t="n">
+        <v>0.527</v>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N45" t="n">
+        <v>62.87</v>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>META</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Meta Platforms, Inc.</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>653.0599999999999</v>
+      </c>
+      <c r="F46" t="n">
+        <v>719.8200000000001</v>
+      </c>
+      <c r="G46" t="n">
+        <v>10.22</v>
+      </c>
+      <c r="H46" t="n">
+        <v>743.6500244140625</v>
+      </c>
+      <c r="I46" t="n">
+        <v>13.86999988555908</v>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K46" t="n">
+        <v>0.791</v>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N46" t="n">
+        <v>81.15000000000001</v>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Tesla, Inc.</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>445.01</v>
+      </c>
+      <c r="F47" t="n">
+        <v>452.26</v>
+      </c>
+      <c r="G47" t="n">
+        <v>1.63</v>
+      </c>
+      <c r="H47" t="n">
+        <v>460.8800048828125</v>
+      </c>
+      <c r="I47" t="n">
+        <v>3.569999933242798</v>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K47" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N47" t="n">
+        <v>66.64</v>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>NVIDIA Corporation</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>184.86</v>
+      </c>
+      <c r="F48" t="n">
+        <v>200.55</v>
+      </c>
+      <c r="G48" t="n">
+        <v>8.49</v>
+      </c>
+      <c r="H48" t="n">
+        <v>190.2700042724609</v>
+      </c>
+      <c r="I48" t="n">
+        <v>2.930000066757202</v>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K48" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N48" t="n">
+        <v>75.23</v>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>JPM</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>JPMorgan Chase &amp; Co.</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>329.19</v>
+      </c>
+      <c r="F49" t="n">
+        <v>344.37</v>
+      </c>
+      <c r="G49" t="n">
+        <v>4.61</v>
+      </c>
+      <c r="H49" t="n">
+        <v>323.0199890136719</v>
+      </c>
+      <c r="I49" t="n">
+        <v>-1.870000004768372</v>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K49" t="n">
+        <v>0.511</v>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N49" t="n">
+        <v>67.14</v>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Visa Inc.</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>349.77</v>
+      </c>
+      <c r="F50" t="n">
+        <v>358.9</v>
+      </c>
+      <c r="G50" t="n">
+        <v>2.61</v>
+      </c>
+      <c r="H50" t="n">
+        <v>352.8500061035156</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0.8799999952316284</v>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K50" t="n">
+        <v>0.637</v>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N50" t="n">
+        <v>66.65000000000001</v>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>JNJ</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Johnson &amp; Johnson</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>204.39</v>
+      </c>
+      <c r="F51" t="n">
+        <v>220.02</v>
+      </c>
+      <c r="G51" t="n">
+        <v>7.65</v>
+      </c>
+      <c r="H51" t="n">
+        <v>216.8500061035156</v>
+      </c>
+      <c r="I51" t="n">
+        <v>6.090000152587891</v>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="K51" t="n">
+        <v>0</v>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>🟢 Buy</t>
+        </is>
+      </c>
+      <c r="N51" t="n">
+        <v>61.47</v>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>WMT</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Walmart Inc.</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>114.53</v>
+      </c>
+      <c r="F52" t="n">
+        <v>117.68</v>
+      </c>
+      <c r="G52" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="H52" t="n">
+        <v>114.1699981689453</v>
+      </c>
+      <c r="I52" t="n">
+        <v>-0.3199999928474426</v>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K52" t="n">
+        <v>0.477</v>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N52" t="n">
+        <v>63.66</v>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>PG</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>The Procter &amp; Gamble Company</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>141.87</v>
+      </c>
+      <c r="F53" t="n">
+        <v>143.69</v>
+      </c>
+      <c r="G53" t="n">
+        <v>1.28</v>
+      </c>
+      <c r="H53" t="n">
+        <v>140.5899963378906</v>
+      </c>
+      <c r="I53" t="n">
+        <v>-0.8999999761581421</v>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="K53" t="n">
+        <v>-0.296</v>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>🟢 Buy</t>
+        </is>
+      </c>
+      <c r="N53" t="n">
+        <v>46.01</v>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>MA</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Mastercard Incorporated</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>575.54</v>
+      </c>
+      <c r="F54" t="n">
+        <v>582.48</v>
+      </c>
+      <c r="G54" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="H54" t="n">
+        <v>554.6599731445312</v>
+      </c>
+      <c r="I54" t="n">
+        <v>-3.630000114440918</v>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K54" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N54" t="n">
+        <v>65.20999999999999</v>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>UNH</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>UnitedHealth Group Incorporated</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>343.98</v>
+      </c>
+      <c r="F55" t="n">
+        <v>316.34</v>
+      </c>
+      <c r="G55" t="n">
+        <v>-8.039999999999999</v>
+      </c>
+      <c r="H55" t="n">
+        <v>402.3500061035156</v>
+      </c>
+      <c r="I55" t="n">
+        <v>16.96999931335449</v>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K55" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N55" t="n">
+        <v>44.75</v>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>HD</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>The Home Depot, Inc.</t>
+        </is>
+      </c>
+      <c r="E56" t="n">
+        <v>374.64</v>
+      </c>
+      <c r="F56" t="n">
+        <v>344.68</v>
+      </c>
+      <c r="G56" t="n">
+        <v>-8</v>
+      </c>
+      <c r="H56" t="n">
+        <v>370.7900085449219</v>
+      </c>
+      <c r="I56" t="n">
+        <v>-1.029999971389771</v>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K56" t="n">
+        <v>0.494</v>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N56" t="n">
+        <v>47.88</v>
+      </c>
+      <c r="O56" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>BAC</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Bank of America Corporation</t>
+        </is>
+      </c>
+      <c r="E57" t="n">
+        <v>55.85</v>
+      </c>
+      <c r="F57" t="n">
+        <v>57.33</v>
+      </c>
+      <c r="G57" t="n">
+        <v>2.65</v>
+      </c>
+      <c r="H57" t="n">
+        <v>55.81000137329102</v>
+      </c>
+      <c r="I57" t="n">
+        <v>-0.07999999821186066</v>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K57" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N57" t="n">
+        <v>67.18000000000001</v>
+      </c>
+      <c r="O57" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>XOM</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Exxon Mobil Corporation</t>
+        </is>
+      </c>
+      <c r="E58" t="n">
+        <v>124.61</v>
+      </c>
+      <c r="F58" t="n">
+        <v>120.45</v>
+      </c>
+      <c r="G58" t="n">
+        <v>-3.34</v>
+      </c>
+      <c r="H58" t="n">
+        <v>109.5400009155273</v>
+      </c>
+      <c r="I58" t="n">
+        <v>-12.09000015258789</v>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K58" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N58" t="n">
+        <v>58.19</v>
+      </c>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>AVGO</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Broadcom Inc.</t>
+        </is>
+      </c>
+      <c r="E59" t="n">
+        <v>344.97</v>
+      </c>
+      <c r="F59" t="n">
+        <v>417.61</v>
+      </c>
+      <c r="G59" t="n">
+        <v>21.06</v>
+      </c>
+      <c r="H59" t="n">
+        <v>324.8200073242188</v>
+      </c>
+      <c r="I59" t="n">
+        <v>-5.840000152587891</v>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K59" t="n">
+        <v>0.382</v>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>🟢 Buy</t>
+        </is>
+      </c>
+      <c r="N59" t="n">
+        <v>87.64</v>
+      </c>
+      <c r="O59" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>COST</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Costco Wholesale Corporation</t>
+        </is>
+      </c>
+      <c r="E60" t="n">
+        <v>924.88</v>
+      </c>
+      <c r="F60" t="n">
+        <v>913.11</v>
+      </c>
+      <c r="G60" t="n">
+        <v>-1.27</v>
+      </c>
+      <c r="H60" t="n">
+        <v>884.47998046875</v>
+      </c>
+      <c r="I60" t="n">
+        <v>-4.369999885559082</v>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K60" t="n">
+        <v>0.823</v>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N60" t="n">
+        <v>64.55</v>
+      </c>
+      <c r="O60" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>2026-01-10</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>PEP</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>PepsiCo, Inc.</t>
+        </is>
+      </c>
+      <c r="E61" t="n">
+        <v>139.91</v>
+      </c>
+      <c r="F61" t="n">
+        <v>146.31</v>
+      </c>
+      <c r="G61" t="n">
+        <v>4.57</v>
+      </c>
+      <c r="H61" t="n">
+        <v>140.4299926757812</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0.3700000047683716</v>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K61" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N61" t="n">
+        <v>65.66</v>
+      </c>
+      <c r="O61" t="inlineStr">
+        <is>
+          <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
📊 Daily StockIQ Insights update (2026-01-11)
</commit_message>
<xml_diff>
--- a/Daily_StockIQ_Insights.xlsx
+++ b/Daily_StockIQ_Insights.xlsx
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O61"/>
+  <dimension ref="A1:O81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4589,6 +4589,1266 @@
       <c r="O61" t="inlineStr">
         <is>
           <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>RELIANCE.NS</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Reliance Industries Limited</t>
+        </is>
+      </c>
+      <c r="E62" t="n">
+        <v>1475.3</v>
+      </c>
+      <c r="F62" t="n">
+        <v>1674.98</v>
+      </c>
+      <c r="G62" t="n">
+        <v>13.53</v>
+      </c>
+      <c r="H62" t="n">
+        <v>1451.489990234375</v>
+      </c>
+      <c r="I62" t="n">
+        <v>-1.610000014305115</v>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K62" t="n">
+        <v>0.735</v>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N62" t="n">
+        <v>85</v>
+      </c>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>TCS.NS</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Tata Consultancy Services Limited</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>3207.8</v>
+      </c>
+      <c r="F63" t="n">
+        <v>3283.32</v>
+      </c>
+      <c r="G63" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="H63" t="n">
+        <v>3398.9599609375</v>
+      </c>
+      <c r="I63" t="n">
+        <v>5.960000038146973</v>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K63" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N63" t="n">
+        <v>62.33</v>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>INFY.NS</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Infosys Limited</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
+        <v>1614.1</v>
+      </c>
+      <c r="F64" t="n">
+        <v>1648.25</v>
+      </c>
+      <c r="G64" t="n">
+        <v>2.12</v>
+      </c>
+      <c r="H64" t="n">
+        <v>1556.349975585938</v>
+      </c>
+      <c r="I64" t="n">
+        <v>-3.579999923706055</v>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K64" t="n">
+        <v>0.633</v>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N64" t="n">
+        <v>65.83</v>
+      </c>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>HDFCBANK.NS</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>HDFC Bank Limited</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>939</v>
+      </c>
+      <c r="F65" t="n">
+        <v>921.17</v>
+      </c>
+      <c r="G65" t="n">
+        <v>-1.9</v>
+      </c>
+      <c r="H65" t="n">
+        <v>949.3800048828125</v>
+      </c>
+      <c r="I65" t="n">
+        <v>1.100000023841858</v>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K65" t="n">
+        <v>0.527</v>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N65" t="n">
+        <v>57.69</v>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>ICICIBANK.NS</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>ICICI Bank Limited</t>
+        </is>
+      </c>
+      <c r="E66" t="n">
+        <v>1404.3</v>
+      </c>
+      <c r="F66" t="n">
+        <v>1322.85</v>
+      </c>
+      <c r="G66" t="n">
+        <v>-5.8</v>
+      </c>
+      <c r="H66" t="n">
+        <v>1479.319946289062</v>
+      </c>
+      <c r="I66" t="n">
+        <v>5.340000152587891</v>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="K66" t="n">
+        <v>-0.65</v>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>❌ Strong Avoid</t>
+        </is>
+      </c>
+      <c r="N66" t="n">
+        <v>28.3</v>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>SBIN.NS</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>State Bank of India</t>
+        </is>
+      </c>
+      <c r="E67" t="n">
+        <v>1000.5</v>
+      </c>
+      <c r="F67" t="n">
+        <v>977.95</v>
+      </c>
+      <c r="G67" t="n">
+        <v>-2.25</v>
+      </c>
+      <c r="H67" t="n">
+        <v>1036.43994140625</v>
+      </c>
+      <c r="I67" t="n">
+        <v>3.589999914169312</v>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="K67" t="n">
+        <v>-0.527</v>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>❌ Strong Avoid</t>
+        </is>
+      </c>
+      <c r="N67" t="n">
+        <v>36.08</v>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>HINDUNILVR.NS</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Hindustan Unilever Limited</t>
+        </is>
+      </c>
+      <c r="E68" t="n">
+        <v>2372.6</v>
+      </c>
+      <c r="F68" t="n">
+        <v>2322.41</v>
+      </c>
+      <c r="G68" t="n">
+        <v>-2.12</v>
+      </c>
+      <c r="H68" t="n">
+        <v>2453.949951171875</v>
+      </c>
+      <c r="I68" t="n">
+        <v>3.430000066757202</v>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K68" t="n">
+        <v>0.681</v>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M68" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N68" t="n">
+        <v>60.45</v>
+      </c>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>ITC.NS</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>ITC Limited</t>
+        </is>
+      </c>
+      <c r="E69" t="n">
+        <v>337.15</v>
+      </c>
+      <c r="F69" t="n">
+        <v>369.51</v>
+      </c>
+      <c r="G69" t="n">
+        <v>9.6</v>
+      </c>
+      <c r="H69" t="n">
+        <v>380.6099853515625</v>
+      </c>
+      <c r="I69" t="n">
+        <v>12.89000034332275</v>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="K69" t="n">
+        <v>-0.459</v>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M69" t="inlineStr">
+        <is>
+          <t>⚠️ Cautious Buy</t>
+        </is>
+      </c>
+      <c r="N69" t="n">
+        <v>55.22</v>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>LT.NS</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Larsen &amp; Toubro Limited</t>
+        </is>
+      </c>
+      <c r="E70" t="n">
+        <v>4025.2</v>
+      </c>
+      <c r="F70" t="n">
+        <v>3957.27</v>
+      </c>
+      <c r="G70" t="n">
+        <v>-1.69</v>
+      </c>
+      <c r="H70" t="n">
+        <v>3036.239990234375</v>
+      </c>
+      <c r="I70" t="n">
+        <v>-24.56999969482422</v>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K70" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N70" t="n">
+        <v>54.27</v>
+      </c>
+      <c r="O70" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>BAJFINANCE.NS</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Bajaj Finance Limited</t>
+        </is>
+      </c>
+      <c r="E71" t="n">
+        <v>959.6</v>
+      </c>
+      <c r="F71" t="n">
+        <v>1026.33</v>
+      </c>
+      <c r="G71" t="n">
+        <v>6.95</v>
+      </c>
+      <c r="H71" t="n">
+        <v>780.7000122070312</v>
+      </c>
+      <c r="I71" t="n">
+        <v>-18.63999938964844</v>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K71" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N71" t="n">
+        <v>73.43000000000001</v>
+      </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>BHARTIARTL.NS</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Bharti Airtel Limited</t>
+        </is>
+      </c>
+      <c r="E72" t="n">
+        <v>2027.1</v>
+      </c>
+      <c r="F72" t="n">
+        <v>2216.93</v>
+      </c>
+      <c r="G72" t="n">
+        <v>9.359999999999999</v>
+      </c>
+      <c r="H72" t="n">
+        <v>2082.75</v>
+      </c>
+      <c r="I72" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K72" t="n">
+        <v>0.625</v>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N72" t="n">
+        <v>76.55</v>
+      </c>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>ASIANPAINT.NS</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>Asian Paints Limited</t>
+        </is>
+      </c>
+      <c r="E73" t="n">
+        <v>2825.5</v>
+      </c>
+      <c r="F73" t="n">
+        <v>2750.07</v>
+      </c>
+      <c r="G73" t="n">
+        <v>-2.67</v>
+      </c>
+      <c r="H73" t="n">
+        <v>2926.580078125</v>
+      </c>
+      <c r="I73" t="n">
+        <v>3.579999923706055</v>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K73" t="n">
+        <v>0.586</v>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N73" t="n">
+        <v>57.72</v>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>AXISBANK.NS</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Axis Bank Limited</t>
+        </is>
+      </c>
+      <c r="E74" t="n">
+        <v>1272</v>
+      </c>
+      <c r="F74" t="n">
+        <v>1200.92</v>
+      </c>
+      <c r="G74" t="n">
+        <v>-5.59</v>
+      </c>
+      <c r="H74" t="n">
+        <v>1132.9599609375</v>
+      </c>
+      <c r="I74" t="n">
+        <v>-10.93000030517578</v>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K74" t="n">
+        <v>0.649</v>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N74" t="n">
+        <v>54.6</v>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>MARUTI.NS</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>Maruti Suzuki India Limited</t>
+        </is>
+      </c>
+      <c r="E75" t="n">
+        <v>16501</v>
+      </c>
+      <c r="F75" t="n">
+        <v>18414.62</v>
+      </c>
+      <c r="G75" t="n">
+        <v>11.6</v>
+      </c>
+      <c r="H75" t="n">
+        <v>17522.169921875</v>
+      </c>
+      <c r="I75" t="n">
+        <v>6.190000057220459</v>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K75" t="n">
+        <v>0.637</v>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N75" t="n">
+        <v>80.14</v>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>SUNPHARMA.NS</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>Sun Pharmaceutical Industries Limited</t>
+        </is>
+      </c>
+      <c r="E76" t="n">
+        <v>1729.9</v>
+      </c>
+      <c r="F76" t="n">
+        <v>1818.45</v>
+      </c>
+      <c r="G76" t="n">
+        <v>5.12</v>
+      </c>
+      <c r="H76" t="n">
+        <v>1696.02001953125</v>
+      </c>
+      <c r="I76" t="n">
+        <v>-1.960000038146973</v>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K76" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N76" t="n">
+        <v>70.68000000000001</v>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>WIPRO.NS</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Wipro Limited</t>
+        </is>
+      </c>
+      <c r="E77" t="n">
+        <v>261.95</v>
+      </c>
+      <c r="F77" t="n">
+        <v>279.99</v>
+      </c>
+      <c r="G77" t="n">
+        <v>6.89</v>
+      </c>
+      <c r="H77" t="n">
+        <v>275.9400024414062</v>
+      </c>
+      <c r="I77" t="n">
+        <v>5.340000152587891</v>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="K77" t="n">
+        <v>-0.65</v>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>⚠️ Cautious Buy</t>
+        </is>
+      </c>
+      <c r="N77" t="n">
+        <v>47.33</v>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>ULTRACEMCO.NS</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>UltraTech Cement Limited</t>
+        </is>
+      </c>
+      <c r="E78" t="n">
+        <v>11937</v>
+      </c>
+      <c r="F78" t="n">
+        <v>11560.26</v>
+      </c>
+      <c r="G78" t="n">
+        <v>-3.16</v>
+      </c>
+      <c r="H78" t="n">
+        <v>10994.83984375</v>
+      </c>
+      <c r="I78" t="n">
+        <v>-7.889999866485596</v>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K78" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M78" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N78" t="n">
+        <v>58.27</v>
+      </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>NTPC.NS</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>NTPC Limited</t>
+        </is>
+      </c>
+      <c r="E79" t="n">
+        <v>336</v>
+      </c>
+      <c r="F79" t="n">
+        <v>328.48</v>
+      </c>
+      <c r="G79" t="n">
+        <v>-2.24</v>
+      </c>
+      <c r="H79" t="n">
+        <v>323.1600036621094</v>
+      </c>
+      <c r="I79" t="n">
+        <v>-3.819999933242798</v>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K79" t="n">
+        <v>0.65</v>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M79" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N79" t="n">
+        <v>59.64</v>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>POWERGRID.NS</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Power Grid Corporation of India Limited</t>
+        </is>
+      </c>
+      <c r="E80" t="n">
+        <v>258</v>
+      </c>
+      <c r="F80" t="n">
+        <v>255.83</v>
+      </c>
+      <c r="G80" t="n">
+        <v>-0.84</v>
+      </c>
+      <c r="H80" t="n">
+        <v>276.9299926757812</v>
+      </c>
+      <c r="I80" t="n">
+        <v>7.340000152587891</v>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K80" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M80" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N80" t="n">
+        <v>62.74</v>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>NSE</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>TITAN.NS</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>Titan Company Limited</t>
+        </is>
+      </c>
+      <c r="E81" t="n">
+        <v>4201.8</v>
+      </c>
+      <c r="F81" t="n">
+        <v>4096.79</v>
+      </c>
+      <c r="G81" t="n">
+        <v>-2.5</v>
+      </c>
+      <c r="H81" t="n">
+        <v>3199.5400390625</v>
+      </c>
+      <c r="I81" t="n">
+        <v>-23.85000038146973</v>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K81" t="n">
+        <v>0.765</v>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M81" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N81" t="n">
+        <v>61.55</v>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
         </is>
       </c>
     </row>
@@ -4603,7 +5863,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6715,6 +7975,636 @@
       <c r="O31" t="inlineStr">
         <is>
           <t>10 Jan 2026, 06:38:26 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>RELIANCE.BO</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Reliance Industries Limited</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>1475.3</v>
+      </c>
+      <c r="F32" t="n">
+        <v>1678.56</v>
+      </c>
+      <c r="G32" t="n">
+        <v>13.78</v>
+      </c>
+      <c r="H32" t="n">
+        <v>1589.280029296875</v>
+      </c>
+      <c r="I32" t="n">
+        <v>7.730000019073486</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K32" t="n">
+        <v>0.883</v>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N32" t="n">
+        <v>88.33</v>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>TCS.BO</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Tata Consultancy Services Limited</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>3208</v>
+      </c>
+      <c r="F33" t="n">
+        <v>3271.49</v>
+      </c>
+      <c r="G33" t="n">
+        <v>1.98</v>
+      </c>
+      <c r="H33" t="n">
+        <v>3355.080078125</v>
+      </c>
+      <c r="I33" t="n">
+        <v>4.579999923706055</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K33" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N33" t="n">
+        <v>61.77</v>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>INFY.BO</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Infosys Limited</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>1614.75</v>
+      </c>
+      <c r="F34" t="n">
+        <v>1666.85</v>
+      </c>
+      <c r="G34" t="n">
+        <v>3.23</v>
+      </c>
+      <c r="H34" t="n">
+        <v>1865.239990234375</v>
+      </c>
+      <c r="I34" t="n">
+        <v>15.51000022888184</v>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K34" t="n">
+        <v>0.633</v>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N34" t="n">
+        <v>67.5</v>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>HDFCBANK.BO</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>HDFC Bank Limited</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>938.7</v>
+      </c>
+      <c r="F35" t="n">
+        <v>925.97</v>
+      </c>
+      <c r="G35" t="n">
+        <v>-1.36</v>
+      </c>
+      <c r="H35" t="n">
+        <v>895.719970703125</v>
+      </c>
+      <c r="I35" t="n">
+        <v>-4.579999923706055</v>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K35" t="n">
+        <v>0.527</v>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N35" t="n">
+        <v>58.51</v>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>ICICIBANK.BO</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>ICICI Bank Limited</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>1403.55</v>
+      </c>
+      <c r="F36" t="n">
+        <v>1330.11</v>
+      </c>
+      <c r="G36" t="n">
+        <v>-5.23</v>
+      </c>
+      <c r="H36" t="n">
+        <v>1372.949951171875</v>
+      </c>
+      <c r="I36" t="n">
+        <v>-2.180000066757202</v>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="K36" t="n">
+        <v>-0.65</v>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>❌ Strong Avoid</t>
+        </is>
+      </c>
+      <c r="N36" t="n">
+        <v>29.15</v>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>SBIN.BO</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>State Bank of India</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>1000</v>
+      </c>
+      <c r="F37" t="n">
+        <v>982.23</v>
+      </c>
+      <c r="G37" t="n">
+        <v>-1.78</v>
+      </c>
+      <c r="H37" t="n">
+        <v>960.75</v>
+      </c>
+      <c r="I37" t="n">
+        <v>-3.930000066757202</v>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="K37" t="n">
+        <v>-0.527</v>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>❌ Strong Avoid</t>
+        </is>
+      </c>
+      <c r="N37" t="n">
+        <v>36.79</v>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>ITC.BO</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>ITC Limited</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>337.1</v>
+      </c>
+      <c r="F38" t="n">
+        <v>370.74</v>
+      </c>
+      <c r="G38" t="n">
+        <v>9.98</v>
+      </c>
+      <c r="H38" t="n">
+        <v>387.1700134277344</v>
+      </c>
+      <c r="I38" t="n">
+        <v>14.85000038146973</v>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="K38" t="n">
+        <v>-0.459</v>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>⚠️ Cautious Buy</t>
+        </is>
+      </c>
+      <c r="N38" t="n">
+        <v>55.79</v>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>LT.BO</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Larsen &amp; Toubro Limited</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>4026.75</v>
+      </c>
+      <c r="F39" t="n">
+        <v>3965.82</v>
+      </c>
+      <c r="G39" t="n">
+        <v>-1.51</v>
+      </c>
+      <c r="H39" t="n">
+        <v>3952.72998046875</v>
+      </c>
+      <c r="I39" t="n">
+        <v>-1.840000033378601</v>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K39" t="n">
+        <v>0.34</v>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N39" t="n">
+        <v>54.53</v>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>AXISBANK.BO</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Axis Bank Limited</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>1271.95</v>
+      </c>
+      <c r="F40" t="n">
+        <v>1217.31</v>
+      </c>
+      <c r="G40" t="n">
+        <v>-4.3</v>
+      </c>
+      <c r="H40" t="n">
+        <v>1326.170043945312</v>
+      </c>
+      <c r="I40" t="n">
+        <v>4.260000228881836</v>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K40" t="n">
+        <v>0.649</v>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N40" t="n">
+        <v>56.54</v>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>BSE</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>MARUTI.BO</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Maruti Suzuki India Limited</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>16501</v>
+      </c>
+      <c r="F41" t="n">
+        <v>18552.39</v>
+      </c>
+      <c r="G41" t="n">
+        <v>12.43</v>
+      </c>
+      <c r="H41" t="n">
+        <v>16643.51953125</v>
+      </c>
+      <c r="I41" t="n">
+        <v>0.8600000143051147</v>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K41" t="n">
+        <v>0.751</v>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N41" t="n">
+        <v>83.67</v>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
         </is>
       </c>
     </row>
@@ -6729,7 +8619,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O61"/>
+  <dimension ref="A1:O81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10874,6 +12764,1266 @@
         </is>
       </c>
     </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Apple Inc.</t>
+        </is>
+      </c>
+      <c r="E62" t="n">
+        <v>259.37</v>
+      </c>
+      <c r="F62" t="n">
+        <v>287.18</v>
+      </c>
+      <c r="G62" t="n">
+        <v>10.72</v>
+      </c>
+      <c r="H62" t="n">
+        <v>256.4400024414062</v>
+      </c>
+      <c r="I62" t="n">
+        <v>-1.129999995231628</v>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="K62" t="n">
+        <v>-0.65</v>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>⚠️ Cautious Buy</t>
+        </is>
+      </c>
+      <c r="N62" t="n">
+        <v>53.08</v>
+      </c>
+      <c r="O62" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>MSFT</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Microsoft Corporation</t>
+        </is>
+      </c>
+      <c r="E63" t="n">
+        <v>479.28</v>
+      </c>
+      <c r="F63" t="n">
+        <v>480.06</v>
+      </c>
+      <c r="G63" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="H63" t="n">
+        <v>468.3699951171875</v>
+      </c>
+      <c r="I63" t="n">
+        <v>-2.279999971389771</v>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K63" t="n">
+        <v>0.296</v>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>🟢 Buy</t>
+        </is>
+      </c>
+      <c r="N63" t="n">
+        <v>56.17</v>
+      </c>
+      <c r="O63" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>GOOGL</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Alphabet Inc.</t>
+        </is>
+      </c>
+      <c r="E64" t="n">
+        <v>328.57</v>
+      </c>
+      <c r="F64" t="n">
+        <v>358.32</v>
+      </c>
+      <c r="G64" t="n">
+        <v>9.050000000000001</v>
+      </c>
+      <c r="H64" t="n">
+        <v>302.1799926757812</v>
+      </c>
+      <c r="I64" t="n">
+        <v>-8.029999732971191</v>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="K64" t="n">
+        <v>-0.6909999999999999</v>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>⚠️ Cautious Buy</t>
+        </is>
+      </c>
+      <c r="N64" t="n">
+        <v>49.76</v>
+      </c>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>AMZN</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Amazon.com, Inc.</t>
+        </is>
+      </c>
+      <c r="E65" t="n">
+        <v>247.38</v>
+      </c>
+      <c r="F65" t="n">
+        <v>251.23</v>
+      </c>
+      <c r="G65" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="H65" t="n">
+        <v>271.4599914550781</v>
+      </c>
+      <c r="I65" t="n">
+        <v>9.729999542236328</v>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K65" t="n">
+        <v>0.527</v>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N65" t="n">
+        <v>62.87</v>
+      </c>
+      <c r="O65" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>META</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Meta Platforms, Inc.</t>
+        </is>
+      </c>
+      <c r="E66" t="n">
+        <v>653.0599999999999</v>
+      </c>
+      <c r="F66" t="n">
+        <v>724.6</v>
+      </c>
+      <c r="G66" t="n">
+        <v>10.95</v>
+      </c>
+      <c r="H66" t="n">
+        <v>703.9099731445312</v>
+      </c>
+      <c r="I66" t="n">
+        <v>7.789999961853027</v>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K66" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N66" t="n">
+        <v>79.63</v>
+      </c>
+      <c r="O66" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>TSLA</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Tesla, Inc.</t>
+        </is>
+      </c>
+      <c r="E67" t="n">
+        <v>445.01</v>
+      </c>
+      <c r="F67" t="n">
+        <v>452.26</v>
+      </c>
+      <c r="G67" t="n">
+        <v>1.63</v>
+      </c>
+      <c r="H67" t="n">
+        <v>519.9000244140625</v>
+      </c>
+      <c r="I67" t="n">
+        <v>16.82999992370605</v>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K67" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N67" t="n">
+        <v>65.84</v>
+      </c>
+      <c r="O67" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>NVDA</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>NVIDIA Corporation</t>
+        </is>
+      </c>
+      <c r="E68" t="n">
+        <v>184.86</v>
+      </c>
+      <c r="F68" t="n">
+        <v>200.53</v>
+      </c>
+      <c r="G68" t="n">
+        <v>8.48</v>
+      </c>
+      <c r="H68" t="n">
+        <v>128.3399963378906</v>
+      </c>
+      <c r="I68" t="n">
+        <v>-30.56999969482422</v>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K68" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M68" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N68" t="n">
+        <v>75.92</v>
+      </c>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>JPM</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>JPMorgan Chase &amp; Co.</t>
+        </is>
+      </c>
+      <c r="E69" t="n">
+        <v>329.19</v>
+      </c>
+      <c r="F69" t="n">
+        <v>343.56</v>
+      </c>
+      <c r="G69" t="n">
+        <v>4.36</v>
+      </c>
+      <c r="H69" t="n">
+        <v>278.5299987792969</v>
+      </c>
+      <c r="I69" t="n">
+        <v>-15.39000034332275</v>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K69" t="n">
+        <v>0.511</v>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M69" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N69" t="n">
+        <v>66.77</v>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Visa Inc.</t>
+        </is>
+      </c>
+      <c r="E70" t="n">
+        <v>349.77</v>
+      </c>
+      <c r="F70" t="n">
+        <v>358.71</v>
+      </c>
+      <c r="G70" t="n">
+        <v>2.56</v>
+      </c>
+      <c r="H70" t="n">
+        <v>339.0299987792969</v>
+      </c>
+      <c r="I70" t="n">
+        <v>-3.069999933242798</v>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K70" t="n">
+        <v>0.637</v>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N70" t="n">
+        <v>66.58</v>
+      </c>
+      <c r="O70" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>JNJ</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Johnson &amp; Johnson</t>
+        </is>
+      </c>
+      <c r="E71" t="n">
+        <v>204.39</v>
+      </c>
+      <c r="F71" t="n">
+        <v>219.95</v>
+      </c>
+      <c r="G71" t="n">
+        <v>7.62</v>
+      </c>
+      <c r="H71" t="n">
+        <v>196.9100036621094</v>
+      </c>
+      <c r="I71" t="n">
+        <v>-3.660000085830688</v>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K71" t="n">
+        <v>0.382</v>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>🟢 Buy</t>
+        </is>
+      </c>
+      <c r="N71" t="n">
+        <v>69.06</v>
+      </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>WMT</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>Walmart Inc.</t>
+        </is>
+      </c>
+      <c r="E72" t="n">
+        <v>114.53</v>
+      </c>
+      <c r="F72" t="n">
+        <v>117.71</v>
+      </c>
+      <c r="G72" t="n">
+        <v>2.78</v>
+      </c>
+      <c r="H72" t="n">
+        <v>102.2799987792969</v>
+      </c>
+      <c r="I72" t="n">
+        <v>-10.69999980926514</v>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K72" t="n">
+        <v>0.477</v>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N72" t="n">
+        <v>63.71</v>
+      </c>
+      <c r="O72" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>PG</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>The Procter &amp; Gamble Company</t>
+        </is>
+      </c>
+      <c r="E73" t="n">
+        <v>141.87</v>
+      </c>
+      <c r="F73" t="n">
+        <v>143.72</v>
+      </c>
+      <c r="G73" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="H73" t="n">
+        <v>150.9600067138672</v>
+      </c>
+      <c r="I73" t="n">
+        <v>6.409999847412109</v>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K73" t="n">
+        <v>0.296</v>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>🟢 Buy</t>
+        </is>
+      </c>
+      <c r="N73" t="n">
+        <v>57.88</v>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>MA</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>Mastercard Incorporated</t>
+        </is>
+      </c>
+      <c r="E74" t="n">
+        <v>575.54</v>
+      </c>
+      <c r="F74" t="n">
+        <v>582.54</v>
+      </c>
+      <c r="G74" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="H74" t="n">
+        <v>590.72998046875</v>
+      </c>
+      <c r="I74" t="n">
+        <v>2.640000104904175</v>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K74" t="n">
+        <v>0.637</v>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N74" t="n">
+        <v>64.56999999999999</v>
+      </c>
+      <c r="O74" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>UNH</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>UnitedHealth Group Incorporated</t>
+        </is>
+      </c>
+      <c r="E75" t="n">
+        <v>343.98</v>
+      </c>
+      <c r="F75" t="n">
+        <v>317.9</v>
+      </c>
+      <c r="G75" t="n">
+        <v>-7.58</v>
+      </c>
+      <c r="H75" t="n">
+        <v>354.5899963378906</v>
+      </c>
+      <c r="I75" t="n">
+        <v>3.079999923706055</v>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K75" t="n">
+        <v>0.827</v>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N75" t="n">
+        <v>55.17</v>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>HD</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>The Home Depot, Inc.</t>
+        </is>
+      </c>
+      <c r="E76" t="n">
+        <v>374.64</v>
+      </c>
+      <c r="F76" t="n">
+        <v>346.03</v>
+      </c>
+      <c r="G76" t="n">
+        <v>-7.64</v>
+      </c>
+      <c r="H76" t="n">
+        <v>357.2300109863281</v>
+      </c>
+      <c r="I76" t="n">
+        <v>-4.650000095367432</v>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K76" t="n">
+        <v>0.494</v>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N76" t="n">
+        <v>48.43</v>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>BAC</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>Bank of America Corporation</t>
+        </is>
+      </c>
+      <c r="E77" t="n">
+        <v>55.85</v>
+      </c>
+      <c r="F77" t="n">
+        <v>57.34</v>
+      </c>
+      <c r="G77" t="n">
+        <v>2.66</v>
+      </c>
+      <c r="H77" t="n">
+        <v>61.02000045776367</v>
+      </c>
+      <c r="I77" t="n">
+        <v>9.260000228881836</v>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K77" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N77" t="n">
+        <v>67.2</v>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>XOM</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>Exxon Mobil Corporation</t>
+        </is>
+      </c>
+      <c r="E78" t="n">
+        <v>124.61</v>
+      </c>
+      <c r="F78" t="n">
+        <v>120.36</v>
+      </c>
+      <c r="G78" t="n">
+        <v>-3.41</v>
+      </c>
+      <c r="H78" t="n">
+        <v>107.8399963378906</v>
+      </c>
+      <c r="I78" t="n">
+        <v>-13.46000003814697</v>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>Negative</t>
+        </is>
+      </c>
+      <c r="K78" t="n">
+        <v>-0.703</v>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M78" t="inlineStr">
+        <is>
+          <t>❌ Strong Avoid</t>
+        </is>
+      </c>
+      <c r="N78" t="n">
+        <v>30.83</v>
+      </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>AVGO</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>Broadcom Inc.</t>
+        </is>
+      </c>
+      <c r="E79" t="n">
+        <v>344.97</v>
+      </c>
+      <c r="F79" t="n">
+        <v>417.76</v>
+      </c>
+      <c r="G79" t="n">
+        <v>21.1</v>
+      </c>
+      <c r="H79" t="n">
+        <v>375.739990234375</v>
+      </c>
+      <c r="I79" t="n">
+        <v>8.920000076293945</v>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K79" t="n">
+        <v>0.382</v>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M79" t="inlineStr">
+        <is>
+          <t>🟢 Buy</t>
+        </is>
+      </c>
+      <c r="N79" t="n">
+        <v>87.64</v>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>COST</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>Costco Wholesale Corporation</t>
+        </is>
+      </c>
+      <c r="E80" t="n">
+        <v>924.88</v>
+      </c>
+      <c r="F80" t="n">
+        <v>912.74</v>
+      </c>
+      <c r="G80" t="n">
+        <v>-1.31</v>
+      </c>
+      <c r="H80" t="n">
+        <v>935.02001953125</v>
+      </c>
+      <c r="I80" t="n">
+        <v>1.100000023841858</v>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K80" t="n">
+        <v>0.572</v>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>Down</t>
+        </is>
+      </c>
+      <c r="M80" t="inlineStr">
+        <is>
+          <t>⚠️ Speculative Buy</t>
+        </is>
+      </c>
+      <c r="N80" t="n">
+        <v>59.47</v>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>2026-01-11</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>NYSE</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>PEP</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>PepsiCo, Inc.</t>
+        </is>
+      </c>
+      <c r="E81" t="n">
+        <v>139.91</v>
+      </c>
+      <c r="F81" t="n">
+        <v>147.33</v>
+      </c>
+      <c r="G81" t="n">
+        <v>5.31</v>
+      </c>
+      <c r="H81" t="n">
+        <v>140.1999969482422</v>
+      </c>
+      <c r="I81" t="n">
+        <v>0.2099999934434891</v>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>Positive</t>
+        </is>
+      </c>
+      <c r="K81" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>Up</t>
+        </is>
+      </c>
+      <c r="M81" t="inlineStr">
+        <is>
+          <t>🚀 Strong Buy</t>
+        </is>
+      </c>
+      <c r="N81" t="n">
+        <v>66.76000000000001</v>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>11 Jan 2026, 06:39:06 PM IST</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>